<commit_message>
Changed template selection logic, added new JSON files, changed the config file
</commit_message>
<xml_diff>
--- a/HumanAssistedResolutionTemplate/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/HumanAssistedResolutionTemplate/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anna.cocan\PycharmProjects\StudioTemplates\HumanAssistedResolutionTemplate\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAC3E14-8433-4449-B80B-AFBACA764E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D19424-AC3D-423C-BA03-99D849437076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -167,9 +167,6 @@
     <t>HumanInTheLoopQueueName</t>
   </si>
   <si>
-    <t>HITLQueue</t>
-  </si>
-  <si>
     <t>Shared</t>
   </si>
   <si>
@@ -203,31 +200,76 @@
     <t>Data post processing started</t>
   </si>
   <si>
-    <t>TaskTitle0</t>
-  </si>
-  <si>
-    <t>TaskCatalog0</t>
-  </si>
-  <si>
-    <t>ERFramework_TaskTitle0</t>
-  </si>
-  <si>
-    <t>ERFramework_TaskCatalog0</t>
-  </si>
-  <si>
     <t>OrchestratorAssetsFolder</t>
   </si>
   <si>
-    <t>TaskTitle1</t>
-  </si>
-  <si>
-    <t>TaskCatalog1</t>
-  </si>
-  <si>
-    <t>ERFramework_TaskTitle1</t>
-  </si>
-  <si>
-    <t>ERFramework_TaskCatalog1</t>
+    <t>TaskCatalog</t>
+  </si>
+  <si>
+    <t>TaskTitle</t>
+  </si>
+  <si>
+    <t>HART_TaskTitle</t>
+  </si>
+  <si>
+    <t>HART_TaskCatalog</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>SolutionDescription</t>
+  </si>
+  <si>
+    <t>HART_Title</t>
+  </si>
+  <si>
+    <t>HART_Description</t>
+  </si>
+  <si>
+    <t>HART_SolutionDescription</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>Detailed description of the exception</t>
+  </si>
+  <si>
+    <t>Description of the steps that should be performed in order to solve the issue</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>System Exception</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>HART_FileName</t>
+  </si>
+  <si>
+    <t>HART.pdf</t>
+  </si>
+  <si>
+    <t>Title of the Action Center Task</t>
+  </si>
+  <si>
+    <t>Catalog of the Action Center Task</t>
+  </si>
+  <si>
+    <t>Title of the exception/case which is displayed in Action Center (used in the 'Create Form Task' activity)</t>
+  </si>
+  <si>
+    <t>Description of the exception/case which is displayed in Action Center (used in the 'Create Form Task' activity)</t>
+  </si>
+  <si>
+    <t>Description of the steps performed to solve the exception/case which is displayed in Action Center (used in the 'Create Form Task' activity)</t>
+  </si>
+  <si>
+    <t>Name of the file displayed in Action Center (used in the 'Create Form Task' activity) The file should be stored in the Storage Bucket</t>
   </si>
 </sst>
 </file>
@@ -603,7 +645,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -697,9 +739,7 @@
       <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>31</v>
       </c>
@@ -709,7 +749,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
@@ -717,18 +757,78 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
@@ -1717,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z977"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1888,34 +1988,34 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1936,10 +2036,10 @@
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
         <v>50</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2903,10 +3003,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA994"/>
+  <dimension ref="A1:AA992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2957,50 +3057,88 @@
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>64</v>
       </c>
-      <c r="C6" t="s">
-        <v>45</v>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3985,8 +4123,6 @@
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated packages to 23.4. Added the user guide.
</commit_message>
<xml_diff>
--- a/HumanAssistedResolutionTemplate/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/HumanAssistedResolutionTemplate/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anna.cocan\PycharmProjects\StudioTemplates\HumanAssistedResolutionTemplate\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9110F98-6563-4B9E-8D33-4D9C35734ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC07D29D-F74B-4E50-A0A5-405456E85F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -134,9 +134,6 @@
     <t>LogMessage_GetTransactionItem</t>
   </si>
   <si>
-    <t>Get Transaction Item started</t>
-  </si>
-  <si>
     <t>Duration, in seconds, between re-execution attempts</t>
   </si>
   <si>
@@ -282,6 +279,33 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>TemplateName</t>
+  </si>
+  <si>
+    <t>Key in the Transaction Item's dictionary that holds the name of the form JSON file, which will be used by the 'Create Form Task' activity.</t>
+  </si>
+  <si>
+    <t>TemplateNameKey</t>
+  </si>
+  <si>
+    <t>Template Name Key</t>
+  </si>
+  <si>
+    <t>LogMessage_TransactionItemNotFound</t>
+  </si>
+  <si>
+    <t>LogMessage_TemplateNameMissingInTransactionItem</t>
+  </si>
+  <si>
+    <t>The transaction item cannot be found.</t>
+  </si>
+  <si>
+    <t>The template name is missing in the transaction item.</t>
+  </si>
+  <si>
+    <t>Get transaction item started</t>
   </si>
 </sst>
 </file>
@@ -656,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="C1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -680,7 +704,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -707,16 +731,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -724,38 +748,38 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -763,27 +787,27 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
@@ -794,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
@@ -805,13 +829,13 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
@@ -819,16 +843,30 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1817,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z977"/>
+  <dimension ref="A1:Z979"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1912,13 +1950,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1929,7 +1967,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1953,101 +1991,115 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B21" t="s">
-        <v>38</v>
+      <c r="B23" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2996,6 +3048,8 @@
     <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3059,44 +3113,44 @@
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3104,41 +3158,41 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>